<commit_message>
- Added ML Sentence Tagger - Fixed a bug when there are no users in rooms and still get IDLENESS alert.
</commit_message>
<xml_diff>
--- a/resources/ety.xlsx
+++ b/resources/ety.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rotemwald/PycharmProjects/FinalProject/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5D8C05-C322-3F4D-976E-E01AB253D52F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="991"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="991" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tsurit- New module boys 2 _onec" sheetId="1" r:id="rId1"/>
@@ -28,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2129" uniqueCount="598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2129" uniqueCount="599">
   <si>
     <t>Line</t>
   </si>
@@ -4188,13 +4194,16 @@
   </si>
   <si>
     <t>Output</t>
+  </si>
+  <si>
+    <t>MAT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Lucida Sans Unicode"/>
@@ -4568,41 +4577,41 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AC322"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="248" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="H1" sqref="A1:AC322"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="0" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="8.5" style="11" customWidth="1"/>
-    <col min="4" max="4" width="8.875" style="11"/>
-    <col min="5" max="5" width="7.625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="11"/>
+    <col min="5" max="5" width="7.6640625" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="14.875" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.6640625" style="12" customWidth="1"/>
     <col min="9" max="9" width="30.5" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="6.625" style="11" customWidth="1"/>
-    <col min="11" max="11" width="6.875" style="11" customWidth="1"/>
-    <col min="12" max="12" width="3.125" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="17" width="4.125" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.6640625" style="11" customWidth="1"/>
+    <col min="11" max="11" width="6.83203125" style="11" customWidth="1"/>
+    <col min="12" max="12" width="3.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="4.1640625" style="11" bestFit="1" customWidth="1"/>
     <col min="18" max="20" width="4.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="29" width="4.125" style="11" bestFit="1" customWidth="1"/>
-    <col min="30" max="16384" width="8.875" style="11"/>
+    <col min="21" max="29" width="4.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4637,7 +4646,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="5" customFormat="1" hidden="1">
+    <row r="2" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2"/>
       <c r="B2" s="2" t="s">
         <v>50</v>
@@ -4659,7 +4668,7 @@
       </c>
       <c r="I2"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>17</v>
       </c>
@@ -4685,13 +4694,13 @@
         <v>58</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K3" s="11">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:12" customFormat="1">
+    <row r="4" spans="1:12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>50</v>
       </c>
@@ -4703,7 +4712,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:12" s="5" customFormat="1" hidden="1">
+    <row r="5" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5"/>
       <c r="B5" s="2" t="s">
         <v>50</v>
@@ -4725,7 +4734,7 @@
       </c>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:12" s="5" customFormat="1" hidden="1">
+    <row r="6" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6"/>
       <c r="B6" s="2" t="s">
         <v>50</v>
@@ -4747,7 +4756,7 @@
       </c>
       <c r="I6"/>
     </row>
-    <row r="7" spans="1:12" hidden="1">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>50</v>
       </c>
@@ -4770,7 +4779,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>18</v>
       </c>
@@ -4796,7 +4805,7 @@
         <v>66</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K8" s="11">
         <v>11</v>
@@ -4805,7 +4814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="5" customFormat="1" hidden="1">
+    <row r="9" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9"/>
       <c r="B9" s="2" t="s">
         <v>50</v>
@@ -4833,7 +4842,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="5" customFormat="1" hidden="1">
+    <row r="10" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10"/>
       <c r="B10" s="2" t="s">
         <v>50</v>
@@ -4857,7 +4866,7 @@
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
     </row>
-    <row r="11" spans="1:12" s="5" customFormat="1" hidden="1">
+    <row r="11" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11"/>
       <c r="B11" s="2" t="s">
         <v>50</v>
@@ -4885,7 +4894,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="5" customFormat="1" hidden="1">
+    <row r="12" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12"/>
       <c r="B12" s="2" t="s">
         <v>50</v>
@@ -4909,7 +4918,7 @@
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
     </row>
-    <row r="13" spans="1:12" s="5" customFormat="1" hidden="1">
+    <row r="13" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13"/>
       <c r="B13" s="2" t="s">
         <v>50</v>
@@ -4936,7 +4945,7 @@
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
     </row>
-    <row r="14" spans="1:12" s="5" customFormat="1" hidden="1">
+    <row r="14" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14"/>
       <c r="B14" s="2" t="s">
         <v>50</v>
@@ -4963,7 +4972,7 @@
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
     </row>
-    <row r="15" spans="1:12" s="5" customFormat="1" hidden="1">
+    <row r="15" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15"/>
       <c r="B15" s="2" t="s">
         <v>50</v>
@@ -4987,7 +4996,7 @@
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
     </row>
-    <row r="16" spans="1:12" s="5" customFormat="1" hidden="1">
+    <row r="16" spans="1:12" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16"/>
       <c r="B16" s="2" t="s">
         <v>50</v>
@@ -5011,7 +5020,7 @@
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
     </row>
-    <row r="17" spans="1:17" s="5" customFormat="1" hidden="1">
+    <row r="17" spans="1:17" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17"/>
       <c r="B17" s="2" t="s">
         <v>50</v>
@@ -5039,7 +5048,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:17" hidden="1">
+    <row r="18" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>50</v>
       </c>
@@ -5064,7 +5073,7 @@
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
     </row>
-    <row r="19" spans="1:17" hidden="1">
+    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>50</v>
       </c>
@@ -5089,7 +5098,7 @@
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
     </row>
-    <row r="20" spans="1:17" s="5" customFormat="1" hidden="1">
+    <row r="20" spans="1:17" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20"/>
       <c r="B20" s="2" t="s">
         <v>50</v>
@@ -5113,7 +5122,7 @@
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
     </row>
-    <row r="21" spans="1:17" s="5" customFormat="1" hidden="1">
+    <row r="21" spans="1:17" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21"/>
       <c r="B21" s="2" t="s">
         <v>50</v>
@@ -5140,7 +5149,7 @@
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
     </row>
-    <row r="22" spans="1:17" s="5" customFormat="1">
+    <row r="22" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>19</v>
       </c>
@@ -5167,7 +5176,7 @@
       </c>
       <c r="I22"/>
       <c r="J22" s="5" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K22" s="5">
         <v>11</v>
@@ -5188,7 +5197,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>20</v>
       </c>
@@ -5214,13 +5223,13 @@
         <v>570</v>
       </c>
       <c r="J23" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K23" s="11">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:17" customFormat="1">
+    <row r="24" spans="1:17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
         <v>50</v>
       </c>
@@ -5232,7 +5241,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:17" s="5" customFormat="1">
+    <row r="25" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>21</v>
       </c>
@@ -5259,7 +5268,7 @@
       </c>
       <c r="I25"/>
       <c r="J25" s="5" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K25" s="5">
         <v>11</v>
@@ -5268,7 +5277,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:17" hidden="1">
+    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
         <v>50</v>
       </c>
@@ -5291,7 +5300,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:17" hidden="1">
+    <row r="27" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
         <v>50</v>
       </c>
@@ -5314,7 +5323,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>22</v>
       </c>
@@ -5340,7 +5349,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="5" customFormat="1" hidden="1">
+    <row r="29" spans="1:17" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29"/>
       <c r="B29" s="2" t="s">
         <v>50</v>
@@ -5362,7 +5371,7 @@
       </c>
       <c r="I29"/>
     </row>
-    <row r="30" spans="1:17" s="5" customFormat="1" hidden="1">
+    <row r="30" spans="1:17" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30"/>
       <c r="B30" s="2" t="s">
         <v>50</v>
@@ -5390,7 +5399,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="5" customFormat="1" hidden="1">
+    <row r="31" spans="1:17" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31"/>
       <c r="B31" s="2" t="s">
         <v>50</v>
@@ -5418,7 +5427,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="5" customFormat="1" hidden="1">
+    <row r="32" spans="1:17" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32"/>
       <c r="B32" s="2" t="s">
         <v>50</v>
@@ -5446,7 +5455,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:21" s="5" customFormat="1" hidden="1">
+    <row r="33" spans="1:21" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33"/>
       <c r="B33" s="2" t="s">
         <v>50</v>
@@ -5474,7 +5483,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:21" s="5" customFormat="1" hidden="1">
+    <row r="34" spans="1:21" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34"/>
       <c r="B34" s="2" t="s">
         <v>50</v>
@@ -5502,7 +5511,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:21" s="5" customFormat="1" hidden="1">
+    <row r="35" spans="1:21" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35"/>
       <c r="B35" s="2" t="s">
         <v>50</v>
@@ -5530,7 +5539,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:21" s="5" customFormat="1" hidden="1">
+    <row r="36" spans="1:21" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36"/>
       <c r="B36" s="2" t="s">
         <v>50</v>
@@ -5558,7 +5567,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:21" s="5" customFormat="1" hidden="1">
+    <row r="37" spans="1:21" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37"/>
       <c r="B37" s="2" t="s">
         <v>50</v>
@@ -5586,7 +5595,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:21" s="5" customFormat="1" hidden="1">
+    <row r="38" spans="1:21" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38"/>
       <c r="B38" s="2" t="s">
         <v>50</v>
@@ -5614,7 +5623,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="25.5">
+    <row r="39" spans="1:21" ht="34" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>23</v>
       </c>
@@ -5640,7 +5649,7 @@
         <v>571</v>
       </c>
       <c r="J39" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K39" s="11">
         <v>11</v>
@@ -5676,7 +5685,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:21" s="5" customFormat="1" hidden="1">
+    <row r="40" spans="1:21" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40"/>
       <c r="B40" s="2" t="s">
         <v>50</v>
@@ -5704,7 +5713,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:21" s="5" customFormat="1" hidden="1">
+    <row r="41" spans="1:21" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41"/>
       <c r="B41" s="2" t="s">
         <v>50</v>
@@ -5726,7 +5735,7 @@
       </c>
       <c r="I41"/>
     </row>
-    <row r="42" spans="1:21" s="5" customFormat="1" hidden="1">
+    <row r="42" spans="1:21" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42"/>
       <c r="B42" s="2" t="s">
         <v>50</v>
@@ -5754,7 +5763,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:21" s="5" customFormat="1" hidden="1">
+    <row r="43" spans="1:21" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43"/>
       <c r="B43" s="2" t="s">
         <v>50</v>
@@ -5776,7 +5785,7 @@
       </c>
       <c r="I43"/>
     </row>
-    <row r="44" spans="1:21" s="5" customFormat="1" hidden="1">
+    <row r="44" spans="1:21" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44"/>
       <c r="B44" s="2" t="s">
         <v>50</v>
@@ -5804,7 +5813,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:21" s="5" customFormat="1" hidden="1">
+    <row r="45" spans="1:21" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45"/>
       <c r="B45" s="2" t="s">
         <v>50</v>
@@ -5826,7 +5835,7 @@
       </c>
       <c r="I45"/>
     </row>
-    <row r="46" spans="1:21" customFormat="1">
+    <row r="46" spans="1:21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B46" s="2" t="s">
         <v>50</v>
       </c>
@@ -5838,7 +5847,7 @@
       <c r="G46" s="1"/>
       <c r="H46" s="3"/>
     </row>
-    <row r="47" spans="1:21" ht="25.5">
+    <row r="47" spans="1:21" ht="34" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>24</v>
       </c>
@@ -5864,7 +5873,7 @@
         <v>572</v>
       </c>
       <c r="J47" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K47" s="11">
         <v>11</v>
@@ -5873,7 +5882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:21">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>25</v>
       </c>
@@ -5899,7 +5908,7 @@
         <v>573</v>
       </c>
       <c r="J48" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K48" s="11">
         <v>11</v>
@@ -5908,7 +5917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:21">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>26</v>
       </c>
@@ -5934,7 +5943,7 @@
         <v>129</v>
       </c>
       <c r="J49" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K49" s="11">
         <v>11</v>
@@ -5943,7 +5952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:21" s="5" customFormat="1" hidden="1">
+    <row r="50" spans="1:21" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50"/>
       <c r="B50" s="2" t="s">
         <v>50</v>
@@ -5965,7 +5974,7 @@
       </c>
       <c r="I50"/>
     </row>
-    <row r="51" spans="1:21" s="5" customFormat="1" hidden="1">
+    <row r="51" spans="1:21" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51"/>
       <c r="B51" s="2" t="s">
         <v>50</v>
@@ -5987,7 +5996,7 @@
       </c>
       <c r="I51"/>
     </row>
-    <row r="52" spans="1:21">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>27</v>
       </c>
@@ -6013,7 +6022,7 @@
         <v>134</v>
       </c>
       <c r="J52" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K52" s="11">
         <v>11</v>
@@ -6022,7 +6031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:21">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>28</v>
       </c>
@@ -6048,7 +6057,7 @@
         <v>137</v>
       </c>
       <c r="J53" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K53" s="11">
         <v>11</v>
@@ -6057,7 +6066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:21" s="5" customFormat="1" hidden="1">
+    <row r="54" spans="1:21" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54"/>
       <c r="B54" s="2" t="s">
         <v>50</v>
@@ -6085,7 +6094,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:21" s="5" customFormat="1" hidden="1">
+    <row r="55" spans="1:21" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55"/>
       <c r="B55" s="2" t="s">
         <v>50</v>
@@ -6113,7 +6122,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:21" s="5" customFormat="1" hidden="1">
+    <row r="56" spans="1:21" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56"/>
       <c r="B56" s="2" t="s">
         <v>50</v>
@@ -6135,7 +6144,7 @@
       </c>
       <c r="I56"/>
     </row>
-    <row r="57" spans="1:21" s="5" customFormat="1" hidden="1">
+    <row r="57" spans="1:21" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57"/>
       <c r="B57" s="2" t="s">
         <v>50</v>
@@ -6163,7 +6172,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:21">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>29</v>
       </c>
@@ -6189,7 +6198,7 @@
         <v>574</v>
       </c>
       <c r="J58" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K58" s="11">
         <v>11</v>
@@ -6222,7 +6231,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:21" s="5" customFormat="1" hidden="1">
+    <row r="59" spans="1:21" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59"/>
       <c r="B59" s="2" t="s">
         <v>50</v>
@@ -6244,7 +6253,7 @@
       </c>
       <c r="I59"/>
     </row>
-    <row r="60" spans="1:21" hidden="1">
+    <row r="60" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
       <c r="B60" s="2" t="s">
         <v>50</v>
       </c>
@@ -6267,7 +6276,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="61" spans="1:21" s="5" customFormat="1" hidden="1">
+    <row r="61" spans="1:21" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61"/>
       <c r="B61" s="2" t="s">
         <v>50</v>
@@ -6292,7 +6301,7 @@
       </c>
       <c r="I61"/>
     </row>
-    <row r="62" spans="1:21" s="5" customFormat="1">
+    <row r="62" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>30</v>
       </c>
@@ -6321,7 +6330,7 @@
         <v>152</v>
       </c>
       <c r="J62" s="5" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K62" s="5">
         <v>11</v>
@@ -6354,7 +6363,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="63" spans="1:21">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>31</v>
       </c>
@@ -6380,13 +6389,13 @@
         <v>155</v>
       </c>
       <c r="J63" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K63" s="11">
         <v>11</v>
       </c>
     </row>
-    <row r="64" spans="1:21" s="5" customFormat="1" hidden="1">
+    <row r="64" spans="1:21" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64"/>
       <c r="B64" s="2" t="s">
         <v>50</v>
@@ -6408,7 +6417,7 @@
       </c>
       <c r="I64"/>
     </row>
-    <row r="65" spans="1:24" s="5" customFormat="1" hidden="1">
+    <row r="65" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65"/>
       <c r="B65" s="2" t="s">
         <v>50</v>
@@ -6436,7 +6445,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:24" s="5" customFormat="1" hidden="1">
+    <row r="66" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66"/>
       <c r="B66" s="2" t="s">
         <v>50</v>
@@ -6464,7 +6473,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:24">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>32</v>
       </c>
@@ -6490,7 +6499,7 @@
         <v>575</v>
       </c>
       <c r="J67" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K67" s="11">
         <v>11</v>
@@ -6505,7 +6514,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="1:24" s="5" customFormat="1" hidden="1">
+    <row r="68" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68"/>
       <c r="B68" s="2" t="s">
         <v>50</v>
@@ -6527,7 +6536,7 @@
       </c>
       <c r="I68"/>
     </row>
-    <row r="69" spans="1:24" s="5" customFormat="1" hidden="1">
+    <row r="69" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69"/>
       <c r="B69" s="2" t="s">
         <v>50</v>
@@ -6549,7 +6558,7 @@
       </c>
       <c r="I69"/>
     </row>
-    <row r="70" spans="1:24" s="5" customFormat="1" hidden="1">
+    <row r="70" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70"/>
       <c r="B70" s="2" t="s">
         <v>50</v>
@@ -6577,7 +6586,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:24" s="5" customFormat="1" hidden="1">
+    <row r="71" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71"/>
       <c r="B71" s="2" t="s">
         <v>50</v>
@@ -6599,7 +6608,7 @@
       </c>
       <c r="I71"/>
     </row>
-    <row r="72" spans="1:24" s="5" customFormat="1" hidden="1">
+    <row r="72" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72"/>
       <c r="B72" s="2" t="s">
         <v>50</v>
@@ -6627,7 +6636,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="1:24" s="5" customFormat="1" hidden="1">
+    <row r="73" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73"/>
       <c r="B73" s="2" t="s">
         <v>50</v>
@@ -6649,7 +6658,7 @@
       </c>
       <c r="I73"/>
     </row>
-    <row r="74" spans="1:24" hidden="1">
+    <row r="74" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
       <c r="B74" s="2" t="s">
         <v>50</v>
       </c>
@@ -6669,7 +6678,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="75" spans="1:24" hidden="1">
+    <row r="75" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
       <c r="B75" s="2" t="s">
         <v>50</v>
       </c>
@@ -6695,7 +6704,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:24" s="5" customFormat="1">
+    <row r="76" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>33</v>
       </c>
@@ -6722,7 +6731,7 @@
       </c>
       <c r="I76"/>
       <c r="J76" s="5" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K76" s="5">
         <v>11</v>
@@ -6764,7 +6773,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="1:24" hidden="1">
+    <row r="77" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
       <c r="B77" s="2" t="s">
         <v>50</v>
       </c>
@@ -6792,7 +6801,7 @@
       <c r="U77" s="5"/>
       <c r="V77" s="5"/>
     </row>
-    <row r="78" spans="1:24" hidden="1">
+    <row r="78" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
       <c r="B78" s="2" t="s">
         <v>50</v>
       </c>
@@ -6812,7 +6821,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="79" spans="1:24" hidden="1">
+    <row r="79" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
       <c r="B79" s="2" t="s">
         <v>50</v>
       </c>
@@ -6838,7 +6847,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="80" spans="1:24" s="5" customFormat="1" hidden="1">
+    <row r="80" spans="1:24" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80"/>
       <c r="B80" s="2" t="s">
         <v>50</v>
@@ -6860,7 +6869,7 @@
       </c>
       <c r="I80"/>
     </row>
-    <row r="81" spans="1:11" s="5" customFormat="1" hidden="1">
+    <row r="81" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81"/>
       <c r="B81" s="2" t="s">
         <v>50</v>
@@ -6882,7 +6891,7 @@
       </c>
       <c r="I81"/>
     </row>
-    <row r="82" spans="1:11">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>70</v>
       </c>
@@ -6908,7 +6917,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="83" spans="1:11" s="5" customFormat="1" hidden="1">
+    <row r="83" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83"/>
       <c r="B83" s="2" t="s">
         <v>50</v>
@@ -6930,7 +6939,7 @@
       </c>
       <c r="I83"/>
     </row>
-    <row r="84" spans="1:11" s="5" customFormat="1" hidden="1">
+    <row r="84" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84"/>
       <c r="B84" s="2" t="s">
         <v>50</v>
@@ -6952,7 +6961,7 @@
       </c>
       <c r="I84"/>
     </row>
-    <row r="85" spans="1:11" s="5" customFormat="1" hidden="1">
+    <row r="85" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85"/>
       <c r="B85" s="2" t="s">
         <v>50</v>
@@ -6974,7 +6983,7 @@
       </c>
       <c r="I85"/>
     </row>
-    <row r="86" spans="1:11" s="5" customFormat="1" hidden="1">
+    <row r="86" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86"/>
       <c r="B86" s="2" t="s">
         <v>50</v>
@@ -6996,7 +7005,7 @@
       </c>
       <c r="I86"/>
     </row>
-    <row r="87" spans="1:11" s="5" customFormat="1" hidden="1">
+    <row r="87" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87"/>
       <c r="B87" s="2" t="s">
         <v>50</v>
@@ -7024,7 +7033,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="88" spans="1:11" s="5" customFormat="1" hidden="1">
+    <row r="88" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88"/>
       <c r="B88" s="2" t="s">
         <v>50</v>
@@ -7046,7 +7055,7 @@
       </c>
       <c r="I88"/>
     </row>
-    <row r="89" spans="1:11" s="5" customFormat="1">
+    <row r="89" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>71</v>
       </c>
@@ -7073,13 +7082,13 @@
       </c>
       <c r="I89"/>
       <c r="J89" s="5" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K89" s="5">
         <v>11</v>
       </c>
     </row>
-    <row r="90" spans="1:11" customFormat="1">
+    <row r="90" spans="1:11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B90" s="2" t="s">
         <v>50</v>
       </c>
@@ -7091,7 +7100,7 @@
       <c r="G90" s="1"/>
       <c r="H90" s="3"/>
     </row>
-    <row r="91" spans="1:11" s="5" customFormat="1" hidden="1">
+    <row r="91" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91"/>
       <c r="B91" s="2" t="s">
         <v>50</v>
@@ -7113,7 +7122,7 @@
       </c>
       <c r="I91"/>
     </row>
-    <row r="92" spans="1:11" s="5" customFormat="1" hidden="1">
+    <row r="92" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92"/>
       <c r="B92" s="2" t="s">
         <v>50</v>
@@ -7141,7 +7150,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:11" s="5" customFormat="1" hidden="1">
+    <row r="93" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93"/>
       <c r="B93" s="2" t="s">
         <v>50</v>
@@ -7163,7 +7172,7 @@
       </c>
       <c r="I93"/>
     </row>
-    <row r="94" spans="1:11" s="5" customFormat="1" hidden="1">
+    <row r="94" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94"/>
       <c r="B94" s="2" t="s">
         <v>50</v>
@@ -7185,7 +7194,7 @@
       </c>
       <c r="I94"/>
     </row>
-    <row r="95" spans="1:11" s="5" customFormat="1" hidden="1">
+    <row r="95" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95"/>
       <c r="B95" s="2" t="s">
         <v>50</v>
@@ -7207,7 +7216,7 @@
       </c>
       <c r="I95"/>
     </row>
-    <row r="96" spans="1:11" s="5" customFormat="1" hidden="1">
+    <row r="96" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96"/>
       <c r="B96" s="2" t="s">
         <v>50</v>
@@ -7229,7 +7238,7 @@
       </c>
       <c r="I96"/>
     </row>
-    <row r="97" spans="1:14" s="5" customFormat="1">
+    <row r="97" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97"/>
       <c r="B97" s="2" t="s">
         <v>50</v>
@@ -7251,7 +7260,7 @@
       </c>
       <c r="I97"/>
     </row>
-    <row r="98" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="98" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98"/>
       <c r="B98" s="2" t="s">
         <v>50</v>
@@ -7273,7 +7282,7 @@
       </c>
       <c r="I98"/>
     </row>
-    <row r="99" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="99" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99"/>
       <c r="B99" s="2" t="s">
         <v>50</v>
@@ -7301,7 +7310,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="100" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="100" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100"/>
       <c r="B100" s="2" t="s">
         <v>50</v>
@@ -7323,7 +7332,7 @@
       </c>
       <c r="I100"/>
     </row>
-    <row r="101" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="101" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101"/>
       <c r="B101" s="2" t="s">
         <v>50</v>
@@ -7345,7 +7354,7 @@
       </c>
       <c r="I101"/>
     </row>
-    <row r="102" spans="1:14" s="5" customFormat="1">
+    <row r="102" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102"/>
       <c r="B102" s="2" t="s">
         <v>50</v>
@@ -7367,7 +7376,7 @@
       </c>
       <c r="I102"/>
     </row>
-    <row r="103" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="103" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103"/>
       <c r="B103" s="2" t="s">
         <v>50</v>
@@ -7389,7 +7398,7 @@
       </c>
       <c r="I103"/>
     </row>
-    <row r="104" spans="1:14">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>73</v>
       </c>
@@ -7415,7 +7424,7 @@
         <v>212</v>
       </c>
       <c r="J104" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K104" s="11">
         <v>11</v>
@@ -7430,7 +7439,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="105" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="105" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105"/>
       <c r="B105" s="2" t="s">
         <v>50</v>
@@ -7458,7 +7467,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="106" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="106" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106"/>
       <c r="B106" s="2" t="s">
         <v>50</v>
@@ -7480,7 +7489,7 @@
       </c>
       <c r="I106"/>
     </row>
-    <row r="107" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="107" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107"/>
       <c r="B107" s="2" t="s">
         <v>50</v>
@@ -7502,7 +7511,7 @@
       </c>
       <c r="I107"/>
     </row>
-    <row r="108" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="108" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108"/>
       <c r="B108" s="2" t="s">
         <v>50</v>
@@ -7530,7 +7539,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="109" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="109" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109"/>
       <c r="B109" s="2" t="s">
         <v>50</v>
@@ -7558,7 +7567,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="110" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="110" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110"/>
       <c r="B110" s="2" t="s">
         <v>50</v>
@@ -7586,7 +7595,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="111" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="111" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111"/>
       <c r="B111" s="2" t="s">
         <v>50</v>
@@ -7614,7 +7623,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="112" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="112" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112"/>
       <c r="B112" s="2" t="s">
         <v>50</v>
@@ -7645,7 +7654,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="113" spans="1:16" s="5" customFormat="1">
+    <row r="113" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>74</v>
       </c>
@@ -7672,7 +7681,7 @@
       </c>
       <c r="I113"/>
       <c r="J113" s="5" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K113" s="5">
         <v>11</v>
@@ -7690,7 +7699,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="114" spans="1:16" s="5" customFormat="1" hidden="1">
+    <row r="114" spans="1:16" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114"/>
       <c r="B114" s="2" t="s">
         <v>50</v>
@@ -7718,7 +7727,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="115" spans="1:16" s="5" customFormat="1" hidden="1">
+    <row r="115" spans="1:16" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115"/>
       <c r="B115" s="2" t="s">
         <v>50</v>
@@ -7740,7 +7749,7 @@
       </c>
       <c r="I115"/>
     </row>
-    <row r="116" spans="1:16" s="5" customFormat="1" hidden="1">
+    <row r="116" spans="1:16" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116"/>
       <c r="B116" s="2" t="s">
         <v>50</v>
@@ -7768,7 +7777,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="117" spans="1:16" s="5" customFormat="1" hidden="1">
+    <row r="117" spans="1:16" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117"/>
       <c r="B117" s="2" t="s">
         <v>50</v>
@@ -7790,7 +7799,7 @@
       </c>
       <c r="I117"/>
     </row>
-    <row r="118" spans="1:16" s="5" customFormat="1" hidden="1">
+    <row r="118" spans="1:16" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118"/>
       <c r="B118" s="2" t="s">
         <v>50</v>
@@ -7818,7 +7827,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="119" spans="1:16" s="5" customFormat="1" hidden="1">
+    <row r="119" spans="1:16" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119"/>
       <c r="B119" s="2" t="s">
         <v>50</v>
@@ -7840,7 +7849,7 @@
       </c>
       <c r="I119"/>
     </row>
-    <row r="120" spans="1:16" s="5" customFormat="1" hidden="1">
+    <row r="120" spans="1:16" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120"/>
       <c r="B120" s="2" t="s">
         <v>50</v>
@@ -7868,7 +7877,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="121" spans="1:16" s="5" customFormat="1" hidden="1">
+    <row r="121" spans="1:16" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121"/>
       <c r="B121" s="2" t="s">
         <v>50</v>
@@ -7890,7 +7899,7 @@
       </c>
       <c r="I121"/>
     </row>
-    <row r="122" spans="1:16" s="5" customFormat="1" hidden="1">
+    <row r="122" spans="1:16" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122"/>
       <c r="B122" s="2" t="s">
         <v>50</v>
@@ -7918,7 +7927,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="123" spans="1:16" hidden="1">
+    <row r="123" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="B123" s="2" t="s">
         <v>50</v>
       </c>
@@ -7941,7 +7950,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="124" spans="1:16" s="5" customFormat="1" hidden="1">
+    <row r="124" spans="1:16" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124"/>
       <c r="B124" s="2" t="s">
         <v>50</v>
@@ -7963,7 +7972,7 @@
       </c>
       <c r="I124"/>
     </row>
-    <row r="125" spans="1:16" s="5" customFormat="1" hidden="1">
+    <row r="125" spans="1:16" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125"/>
       <c r="B125" s="2" t="s">
         <v>50</v>
@@ -7991,7 +8000,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="126" spans="1:16" s="5" customFormat="1" hidden="1">
+    <row r="126" spans="1:16" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126"/>
       <c r="B126" s="2" t="s">
         <v>50</v>
@@ -8013,7 +8022,7 @@
       </c>
       <c r="I126"/>
     </row>
-    <row r="127" spans="1:16" s="5" customFormat="1" hidden="1">
+    <row r="127" spans="1:16" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127"/>
       <c r="B127" s="2" t="s">
         <v>50</v>
@@ -8041,7 +8050,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="128" spans="1:16" s="5" customFormat="1" hidden="1">
+    <row r="128" spans="1:16" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128"/>
       <c r="B128" s="2" t="s">
         <v>50</v>
@@ -8063,7 +8072,7 @@
       </c>
       <c r="I128"/>
     </row>
-    <row r="129" spans="1:25" s="5" customFormat="1" hidden="1">
+    <row r="129" spans="1:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129"/>
       <c r="B129" s="2" t="s">
         <v>50</v>
@@ -8091,7 +8100,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="130" spans="1:25" s="5" customFormat="1" hidden="1">
+    <row r="130" spans="1:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130"/>
       <c r="B130" s="2" t="s">
         <v>50</v>
@@ -8113,7 +8122,7 @@
       </c>
       <c r="I130"/>
     </row>
-    <row r="131" spans="1:25" s="5" customFormat="1" hidden="1">
+    <row r="131" spans="1:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131"/>
       <c r="B131" s="2" t="s">
         <v>50</v>
@@ -8135,7 +8144,7 @@
       </c>
       <c r="I131"/>
     </row>
-    <row r="132" spans="1:25" s="5" customFormat="1" hidden="1">
+    <row r="132" spans="1:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132"/>
       <c r="B132" s="2" t="s">
         <v>50</v>
@@ -8157,7 +8166,7 @@
       </c>
       <c r="I132"/>
     </row>
-    <row r="133" spans="1:25" ht="25.5">
+    <row r="133" spans="1:25" ht="34" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>77</v>
       </c>
@@ -8183,7 +8192,7 @@
         <v>582</v>
       </c>
       <c r="J133" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K133" s="11">
         <v>11</v>
@@ -8231,7 +8240,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="134" spans="1:25" ht="25.5">
+    <row r="134" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>89</v>
       </c>
@@ -8257,13 +8266,13 @@
         <v>253</v>
       </c>
       <c r="J134" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K134" s="11">
         <v>11</v>
       </c>
     </row>
-    <row r="135" spans="1:25" s="5" customFormat="1" hidden="1">
+    <row r="135" spans="1:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135"/>
       <c r="B135" s="2" t="s">
         <v>50</v>
@@ -8285,7 +8294,7 @@
       </c>
       <c r="I135"/>
     </row>
-    <row r="136" spans="1:25" s="5" customFormat="1" hidden="1">
+    <row r="136" spans="1:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136"/>
       <c r="B136" s="2" t="s">
         <v>50</v>
@@ -8313,7 +8322,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="137" spans="1:25" s="5" customFormat="1" hidden="1">
+    <row r="137" spans="1:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137"/>
       <c r="B137" s="2" t="s">
         <v>50</v>
@@ -8341,7 +8350,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="138" spans="1:25" s="5" customFormat="1" hidden="1">
+    <row r="138" spans="1:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138"/>
       <c r="B138" s="2" t="s">
         <v>50</v>
@@ -8369,7 +8378,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="139" spans="1:25" s="5" customFormat="1" hidden="1">
+    <row r="139" spans="1:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139"/>
       <c r="B139" s="2" t="s">
         <v>50</v>
@@ -8397,7 +8406,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="140" spans="1:25">
+    <row r="140" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>90</v>
       </c>
@@ -8426,7 +8435,7 @@
         <v>263</v>
       </c>
       <c r="J140" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K140" s="11">
         <v>11</v>
@@ -8453,7 +8462,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="141" spans="1:25" s="5" customFormat="1" hidden="1">
+    <row r="141" spans="1:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141"/>
       <c r="B141" s="2" t="s">
         <v>50</v>
@@ -8481,7 +8490,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="1:25" s="5" customFormat="1" hidden="1">
+    <row r="142" spans="1:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142"/>
       <c r="B142" s="2" t="s">
         <v>50</v>
@@ -8509,7 +8518,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:25" s="5" customFormat="1" hidden="1">
+    <row r="143" spans="1:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143"/>
       <c r="B143" s="2" t="s">
         <v>50</v>
@@ -8537,7 +8546,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:25" s="5" customFormat="1" hidden="1">
+    <row r="144" spans="1:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144"/>
       <c r="B144" s="2" t="s">
         <v>50</v>
@@ -8565,7 +8574,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:22" s="5" customFormat="1" hidden="1">
+    <row r="145" spans="1:22" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145"/>
       <c r="B145" s="2" t="s">
         <v>50</v>
@@ -8593,7 +8602,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="146" spans="1:22" s="5" customFormat="1" hidden="1">
+    <row r="146" spans="1:22" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146"/>
       <c r="B146" s="2" t="s">
         <v>50</v>
@@ -8621,7 +8630,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:22" s="5" customFormat="1" hidden="1">
+    <row r="147" spans="1:22" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147"/>
       <c r="B147" s="2" t="s">
         <v>50</v>
@@ -8649,7 +8658,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="148" spans="1:22" s="5" customFormat="1" hidden="1">
+    <row r="148" spans="1:22" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148"/>
       <c r="B148" s="2" t="s">
         <v>50</v>
@@ -8677,7 +8686,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="149" spans="1:22" s="5" customFormat="1" ht="25.5">
+    <row r="149" spans="1:22" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>91</v>
       </c>
@@ -8704,7 +8713,7 @@
       </c>
       <c r="I149"/>
       <c r="J149" s="5" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K149" s="5">
         <v>11</v>
@@ -8743,7 +8752,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="150" spans="1:22" s="5" customFormat="1" hidden="1">
+    <row r="150" spans="1:22" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150"/>
       <c r="B150" s="2" t="s">
         <v>50</v>
@@ -8765,7 +8774,7 @@
       </c>
       <c r="I150"/>
     </row>
-    <row r="151" spans="1:22" hidden="1">
+    <row r="151" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="B151" s="2" t="s">
         <v>50</v>
       </c>
@@ -8788,7 +8797,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="152" spans="1:22" s="5" customFormat="1" hidden="1">
+    <row r="152" spans="1:22" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152"/>
       <c r="B152" s="2" t="s">
         <v>50</v>
@@ -8810,7 +8819,7 @@
       </c>
       <c r="I152"/>
     </row>
-    <row r="153" spans="1:22" s="5" customFormat="1" hidden="1">
+    <row r="153" spans="1:22" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153"/>
       <c r="B153" s="2" t="s">
         <v>50</v>
@@ -8832,7 +8841,7 @@
       </c>
       <c r="I153"/>
     </row>
-    <row r="154" spans="1:22" s="5" customFormat="1" hidden="1">
+    <row r="154" spans="1:22" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154"/>
       <c r="B154" s="2" t="s">
         <v>50</v>
@@ -8854,7 +8863,7 @@
       </c>
       <c r="I154"/>
     </row>
-    <row r="155" spans="1:22" hidden="1">
+    <row r="155" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="B155" s="2" t="s">
         <v>50</v>
       </c>
@@ -8877,7 +8886,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="156" spans="1:22" hidden="1">
+    <row r="156" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="B156" s="2" t="s">
         <v>50</v>
       </c>
@@ -8900,7 +8909,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="157" spans="1:22" s="5" customFormat="1" hidden="1">
+    <row r="157" spans="1:22" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157"/>
       <c r="B157" s="2" t="s">
         <v>50</v>
@@ -8922,7 +8931,7 @@
       </c>
       <c r="I157"/>
     </row>
-    <row r="158" spans="1:22" ht="25.5">
+    <row r="158" spans="1:22" ht="34" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>92</v>
       </c>
@@ -8948,7 +8957,7 @@
         <v>288</v>
       </c>
       <c r="J158" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K158" s="11">
         <v>11</v>
@@ -8963,7 +8972,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="159" spans="1:22" customFormat="1">
+    <row r="159" spans="1:22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B159" s="2" t="s">
         <v>50</v>
       </c>
@@ -8975,7 +8984,7 @@
       <c r="G159" s="1"/>
       <c r="H159" s="3"/>
     </row>
-    <row r="160" spans="1:22" hidden="1">
+    <row r="160" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="B160" s="2" t="s">
         <v>50</v>
       </c>
@@ -8995,7 +9004,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="161" spans="1:14" hidden="1">
+    <row r="161" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B161" s="2" t="s">
         <v>50</v>
       </c>
@@ -9015,7 +9024,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="162" spans="1:14" hidden="1">
+    <row r="162" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B162" s="2" t="s">
         <v>50</v>
       </c>
@@ -9041,7 +9050,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="163" spans="1:14" hidden="1">
+    <row r="163" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B163" s="2" t="s">
         <v>50</v>
       </c>
@@ -9067,7 +9076,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="164" spans="1:14" hidden="1">
+    <row r="164" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B164" s="2" t="s">
         <v>50</v>
       </c>
@@ -9093,7 +9102,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="165" spans="1:14" hidden="1">
+    <row r="165" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B165" s="2" t="s">
         <v>50</v>
       </c>
@@ -9119,7 +9128,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="166" spans="1:14" s="5" customFormat="1">
+    <row r="166" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>93</v>
       </c>
@@ -9146,7 +9155,7 @@
       </c>
       <c r="I166"/>
       <c r="J166" s="5" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K166" s="5">
         <v>11</v>
@@ -9155,7 +9164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:14" s="5" customFormat="1">
+    <row r="167" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>94</v>
       </c>
@@ -9182,7 +9191,7 @@
       </c>
       <c r="I167"/>
       <c r="J167" s="5" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K167" s="5">
         <v>11</v>
@@ -9197,7 +9206,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="168" spans="1:14" customFormat="1">
+    <row r="168" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B168" s="2" t="s">
         <v>50</v>
       </c>
@@ -9209,7 +9218,7 @@
       <c r="G168" s="1"/>
       <c r="H168" s="3"/>
     </row>
-    <row r="169" spans="1:14" ht="38.25">
+    <row r="169" spans="1:14" ht="51" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>95</v>
       </c>
@@ -9238,7 +9247,7 @@
         <v>302</v>
       </c>
       <c r="J169" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K169" s="11">
         <v>11</v>
@@ -9247,7 +9256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="170" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170"/>
       <c r="B170" s="2" t="s">
         <v>50</v>
@@ -9269,7 +9278,7 @@
       </c>
       <c r="I170"/>
     </row>
-    <row r="171" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="171" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171"/>
       <c r="B171" s="2" t="s">
         <v>50</v>
@@ -9291,7 +9300,7 @@
       </c>
       <c r="I171"/>
     </row>
-    <row r="172" spans="1:14" hidden="1">
+    <row r="172" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B172" s="2" t="s">
         <v>50</v>
       </c>
@@ -9314,7 +9323,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="173" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="173" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173"/>
       <c r="B173" s="2" t="s">
         <v>50</v>
@@ -9336,7 +9345,7 @@
       </c>
       <c r="I173"/>
     </row>
-    <row r="174" spans="1:14">
+    <row r="174" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>96</v>
       </c>
@@ -9362,7 +9371,7 @@
         <v>310</v>
       </c>
       <c r="J174" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K174" s="11">
         <v>11</v>
@@ -9371,7 +9380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:14">
+    <row r="175" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>97</v>
       </c>
@@ -9397,7 +9406,7 @@
         <v>313</v>
       </c>
       <c r="J175" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K175" s="11">
         <v>11</v>
@@ -9406,7 +9415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="176" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176"/>
       <c r="B176" s="2" t="s">
         <v>50</v>
@@ -9428,7 +9437,7 @@
       </c>
       <c r="I176"/>
     </row>
-    <row r="177" spans="1:26">
+    <row r="177" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>98</v>
       </c>
@@ -9454,7 +9463,7 @@
         <v>317</v>
       </c>
       <c r="J177" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K177" s="11">
         <v>11</v>
@@ -9463,7 +9472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:26" s="5" customFormat="1" hidden="1">
+    <row r="178" spans="1:26" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178"/>
       <c r="B178" s="2" t="s">
         <v>50</v>
@@ -9485,7 +9494,7 @@
       </c>
       <c r="I178"/>
     </row>
-    <row r="179" spans="1:26" ht="38.25">
+    <row r="179" spans="1:26" ht="51" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>99</v>
       </c>
@@ -9511,7 +9520,7 @@
         <v>322</v>
       </c>
       <c r="J179" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K179" s="11">
         <v>11</v>
@@ -9556,7 +9565,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="180" spans="1:26" customFormat="1">
+    <row r="180" spans="1:26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B180" s="2" t="s">
         <v>50</v>
       </c>
@@ -9568,7 +9577,7 @@
       <c r="G180" s="1"/>
       <c r="H180" s="3"/>
     </row>
-    <row r="181" spans="1:26" s="5" customFormat="1" ht="25.5">
+    <row r="181" spans="1:26" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>100</v>
       </c>
@@ -9595,7 +9604,7 @@
       </c>
       <c r="I181"/>
       <c r="J181" s="5" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K181" s="5">
         <v>11</v>
@@ -9604,7 +9613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:26" s="5" customFormat="1">
+    <row r="182" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>101</v>
       </c>
@@ -9631,7 +9640,7 @@
       </c>
       <c r="I182"/>
       <c r="J182" s="5" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K182" s="5">
         <v>11</v>
@@ -9682,7 +9691,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="183" spans="1:26" s="5" customFormat="1" hidden="1">
+    <row r="183" spans="1:26" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183"/>
       <c r="B183" s="2" t="s">
         <v>50</v>
@@ -9704,7 +9713,7 @@
       </c>
       <c r="I183"/>
     </row>
-    <row r="184" spans="1:26" s="5" customFormat="1" hidden="1">
+    <row r="184" spans="1:26" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184"/>
       <c r="B184" s="2" t="s">
         <v>50</v>
@@ -9732,7 +9741,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="185" spans="1:26" s="5" customFormat="1" hidden="1">
+    <row r="185" spans="1:26" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185"/>
       <c r="B185" s="2" t="s">
         <v>50</v>
@@ -9760,7 +9769,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="186" spans="1:26" s="5" customFormat="1" hidden="1">
+    <row r="186" spans="1:26" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186"/>
       <c r="B186" s="2" t="s">
         <v>50</v>
@@ -9788,7 +9797,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="187" spans="1:26" s="5" customFormat="1" hidden="1">
+    <row r="187" spans="1:26" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187"/>
       <c r="B187" s="2" t="s">
         <v>50</v>
@@ -9816,7 +9825,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="188" spans="1:26">
+    <row r="188" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>102</v>
       </c>
@@ -9842,7 +9851,7 @@
         <v>584</v>
       </c>
       <c r="J188" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K188" s="11">
         <v>11</v>
@@ -9851,7 +9860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:26" s="5" customFormat="1" hidden="1">
+    <row r="189" spans="1:26" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189"/>
       <c r="B189" s="2" t="s">
         <v>50</v>
@@ -9873,7 +9882,7 @@
       </c>
       <c r="I189"/>
     </row>
-    <row r="190" spans="1:26" hidden="1">
+    <row r="190" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
       <c r="B190" s="2" t="s">
         <v>50</v>
       </c>
@@ -9896,7 +9905,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="191" spans="1:26" s="5" customFormat="1" hidden="1">
+    <row r="191" spans="1:26" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191"/>
       <c r="B191" s="2" t="s">
         <v>50</v>
@@ -9918,7 +9927,7 @@
       </c>
       <c r="I191"/>
     </row>
-    <row r="192" spans="1:26" s="5" customFormat="1" hidden="1">
+    <row r="192" spans="1:26" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192"/>
       <c r="B192" s="2" t="s">
         <v>50</v>
@@ -9940,7 +9949,7 @@
       </c>
       <c r="I192"/>
     </row>
-    <row r="193" spans="1:17" s="5" customFormat="1" hidden="1">
+    <row r="193" spans="1:17" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193"/>
       <c r="B193" s="2" t="s">
         <v>50</v>
@@ -9962,7 +9971,7 @@
       </c>
       <c r="I193"/>
     </row>
-    <row r="194" spans="1:17" hidden="1">
+    <row r="194" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B194" s="2" t="s">
         <v>50</v>
       </c>
@@ -9985,7 +9994,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="195" spans="1:17" s="5" customFormat="1" hidden="1">
+    <row r="195" spans="1:17" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195"/>
       <c r="B195" s="2" t="s">
         <v>50</v>
@@ -10007,7 +10016,7 @@
       </c>
       <c r="I195"/>
     </row>
-    <row r="196" spans="1:17" s="5" customFormat="1" hidden="1">
+    <row r="196" spans="1:17" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196"/>
       <c r="B196" s="2" t="s">
         <v>50</v>
@@ -10029,7 +10038,7 @@
       </c>
       <c r="I196"/>
     </row>
-    <row r="197" spans="1:17" s="5" customFormat="1" hidden="1">
+    <row r="197" spans="1:17" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197"/>
       <c r="B197" s="2" t="s">
         <v>50</v>
@@ -10051,7 +10060,7 @@
       </c>
       <c r="I197"/>
     </row>
-    <row r="198" spans="1:17" s="5" customFormat="1" hidden="1">
+    <row r="198" spans="1:17" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198"/>
       <c r="B198" s="2" t="s">
         <v>50</v>
@@ -10073,7 +10082,7 @@
       </c>
       <c r="I198"/>
     </row>
-    <row r="199" spans="1:17" ht="25.5">
+    <row r="199" spans="1:17" ht="34" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>103</v>
       </c>
@@ -10102,7 +10111,7 @@
         <v>356</v>
       </c>
       <c r="J199" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K199" s="11">
         <v>11</v>
@@ -10111,7 +10120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:17" ht="25.5">
+    <row r="200" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>104</v>
       </c>
@@ -10137,7 +10146,7 @@
         <v>359</v>
       </c>
       <c r="J200" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K200" s="11">
         <v>11</v>
@@ -10161,7 +10170,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="201" spans="1:17" s="5" customFormat="1">
+    <row r="201" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>105</v>
       </c>
@@ -10188,13 +10197,13 @@
       </c>
       <c r="I201"/>
       <c r="J201" s="5" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K201" s="5">
         <v>11</v>
       </c>
     </row>
-    <row r="202" spans="1:17" customFormat="1">
+    <row r="202" spans="1:17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B202" s="2" t="s">
         <v>50</v>
       </c>
@@ -10206,7 +10215,7 @@
       <c r="G202" s="1"/>
       <c r="H202" s="3"/>
     </row>
-    <row r="203" spans="1:17" s="5" customFormat="1" hidden="1">
+    <row r="203" spans="1:17" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203"/>
       <c r="B203" s="2" t="s">
         <v>50</v>
@@ -10228,7 +10237,7 @@
       </c>
       <c r="I203"/>
     </row>
-    <row r="204" spans="1:17" s="5" customFormat="1" hidden="1">
+    <row r="204" spans="1:17" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204"/>
       <c r="B204" s="2" t="s">
         <v>50</v>
@@ -10250,7 +10259,7 @@
       </c>
       <c r="I204"/>
     </row>
-    <row r="205" spans="1:17" s="5" customFormat="1" hidden="1">
+    <row r="205" spans="1:17" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205"/>
       <c r="B205" s="2" t="s">
         <v>50</v>
@@ -10272,7 +10281,7 @@
       </c>
       <c r="I205"/>
     </row>
-    <row r="206" spans="1:17" s="5" customFormat="1" hidden="1">
+    <row r="206" spans="1:17" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206"/>
       <c r="B206" s="2" t="s">
         <v>50</v>
@@ -10294,7 +10303,7 @@
       </c>
       <c r="I206"/>
     </row>
-    <row r="207" spans="1:17" s="5" customFormat="1">
+    <row r="207" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A207"/>
       <c r="B207" s="2" t="s">
         <v>50</v>
@@ -10316,7 +10325,7 @@
       </c>
       <c r="I207"/>
     </row>
-    <row r="208" spans="1:17" s="5" customFormat="1">
+    <row r="208" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A208"/>
       <c r="B208" s="2" t="s">
         <v>50</v>
@@ -10338,7 +10347,7 @@
       </c>
       <c r="I208"/>
     </row>
-    <row r="209" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="209" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209"/>
       <c r="B209" s="2" t="s">
         <v>50</v>
@@ -10360,7 +10369,7 @@
       </c>
       <c r="I209"/>
     </row>
-    <row r="210" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="210" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A210"/>
       <c r="B210" s="2" t="s">
         <v>50</v>
@@ -10382,7 +10391,7 @@
       </c>
       <c r="I210"/>
     </row>
-    <row r="211" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="211" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A211"/>
       <c r="B211" s="2" t="s">
         <v>50</v>
@@ -10404,7 +10413,7 @@
       </c>
       <c r="I211"/>
     </row>
-    <row r="212" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="212" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A212"/>
       <c r="B212" s="2" t="s">
         <v>50</v>
@@ -10426,7 +10435,7 @@
       </c>
       <c r="I212"/>
     </row>
-    <row r="213" spans="1:14" s="5" customFormat="1">
+    <row r="213" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A213"/>
       <c r="B213" s="2" t="s">
         <v>50</v>
@@ -10448,7 +10457,7 @@
       </c>
       <c r="I213"/>
     </row>
-    <row r="214" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="214" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214"/>
       <c r="B214" s="2" t="s">
         <v>50</v>
@@ -10470,7 +10479,7 @@
       </c>
       <c r="I214"/>
     </row>
-    <row r="215" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="215" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215"/>
       <c r="B215" s="2" t="s">
         <v>50</v>
@@ -10492,7 +10501,7 @@
       </c>
       <c r="I215"/>
     </row>
-    <row r="216" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="216" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216"/>
       <c r="B216" s="2" t="s">
         <v>50</v>
@@ -10520,7 +10529,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="217" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="217" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A217"/>
       <c r="B217" s="2" t="s">
         <v>50</v>
@@ -10542,7 +10551,7 @@
       </c>
       <c r="I217"/>
     </row>
-    <row r="218" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="218" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A218"/>
       <c r="B218" s="2" t="s">
         <v>50</v>
@@ -10570,7 +10579,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="219" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="219" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219"/>
       <c r="B219" s="2" t="s">
         <v>50</v>
@@ -10598,7 +10607,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="220" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="220" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220"/>
       <c r="B220" s="2" t="s">
         <v>50</v>
@@ -10626,7 +10635,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="221" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="221" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221"/>
       <c r="B221" s="2" t="s">
         <v>50</v>
@@ -10648,7 +10657,7 @@
       </c>
       <c r="I221"/>
     </row>
-    <row r="222" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="222" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222"/>
       <c r="B222" s="2" t="s">
         <v>50</v>
@@ -10676,7 +10685,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="223" spans="1:14">
+    <row r="223" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>106</v>
       </c>
@@ -10702,7 +10711,7 @@
         <v>585</v>
       </c>
       <c r="J223" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K223" s="11">
         <v>11</v>
@@ -10714,7 +10723,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="224" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="224" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224"/>
       <c r="B224" s="2" t="s">
         <v>50</v>
@@ -10742,7 +10751,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="225" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="225" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A225"/>
       <c r="B225" s="2" t="s">
         <v>50</v>
@@ -10770,7 +10779,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="226" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="226" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A226"/>
       <c r="B226" s="2" t="s">
         <v>50</v>
@@ -10798,7 +10807,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="227" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="227" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A227"/>
       <c r="B227" s="2" t="s">
         <v>50</v>
@@ -10826,7 +10835,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="228" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="228" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A228"/>
       <c r="B228" s="2" t="s">
         <v>50</v>
@@ -10854,7 +10863,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="229" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="229" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A229"/>
       <c r="B229" s="2" t="s">
         <v>50</v>
@@ -10882,7 +10891,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="230" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="230" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A230"/>
       <c r="B230" s="2" t="s">
         <v>50</v>
@@ -10910,7 +10919,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="231" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="231" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A231"/>
       <c r="B231" s="2" t="s">
         <v>50</v>
@@ -10938,7 +10947,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="232" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="232" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A232"/>
       <c r="B232" s="2" t="s">
         <v>50</v>
@@ -10966,7 +10975,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="233" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="233" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A233"/>
       <c r="B233" s="2" t="s">
         <v>50</v>
@@ -10994,7 +11003,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="234" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="234" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A234"/>
       <c r="B234" s="2" t="s">
         <v>50</v>
@@ -11022,7 +11031,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="235" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="235" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A235"/>
       <c r="B235" s="2" t="s">
         <v>50</v>
@@ -11050,7 +11059,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="236" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="236" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A236"/>
       <c r="B236" s="2" t="s">
         <v>50</v>
@@ -11078,7 +11087,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="237" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="237" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A237"/>
       <c r="B237" s="2" t="s">
         <v>50</v>
@@ -11106,7 +11115,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="238" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="238" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A238"/>
       <c r="B238" s="2" t="s">
         <v>50</v>
@@ -11134,7 +11143,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="239" spans="1:14" s="5" customFormat="1">
+    <row r="239" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>107</v>
       </c>
@@ -11161,7 +11170,7 @@
       </c>
       <c r="I239"/>
       <c r="J239" s="5" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K239" s="5">
         <v>11</v>
@@ -11176,7 +11185,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="240" spans="1:14" customFormat="1">
+    <row r="240" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B240" s="2" t="s">
         <v>50</v>
       </c>
@@ -11188,7 +11197,7 @@
       <c r="G240" s="1"/>
       <c r="H240" s="3"/>
     </row>
-    <row r="241" spans="1:14" ht="25.5">
+    <row r="241" spans="1:14" ht="34" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>109</v>
       </c>
@@ -11214,7 +11223,7 @@
         <v>406</v>
       </c>
       <c r="J241" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K241" s="11">
         <v>11</v>
@@ -11226,7 +11235,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="242" spans="1:14" ht="25.5">
+    <row r="242" spans="1:14" ht="34" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>110</v>
       </c>
@@ -11252,7 +11261,7 @@
         <v>586</v>
       </c>
       <c r="J242" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K242" s="11">
         <v>11</v>
@@ -11264,7 +11273,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="243" spans="1:14" s="5" customFormat="1" ht="25.5">
+    <row r="243" spans="1:14" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>111</v>
       </c>
@@ -11291,7 +11300,7 @@
       </c>
       <c r="I243"/>
       <c r="J243" s="5" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K243" s="5">
         <v>11</v>
@@ -11306,7 +11315,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="244" spans="1:14">
+    <row r="244" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>112</v>
       </c>
@@ -11332,7 +11341,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="245" spans="1:14">
+    <row r="245" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>113</v>
       </c>
@@ -11358,7 +11367,7 @@
         <v>414</v>
       </c>
       <c r="J245" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K245" s="11">
         <v>11</v>
@@ -11367,7 +11376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="246" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A246"/>
       <c r="B246" s="2" t="s">
         <v>50</v>
@@ -11389,7 +11398,7 @@
       </c>
       <c r="I246"/>
     </row>
-    <row r="247" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="247" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A247"/>
       <c r="B247" s="2" t="s">
         <v>50</v>
@@ -11417,7 +11426,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="248" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="248" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A248"/>
       <c r="B248" s="2" t="s">
         <v>50</v>
@@ -11445,7 +11454,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="249" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="249" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A249"/>
       <c r="B249" s="2" t="s">
         <v>50</v>
@@ -11473,7 +11482,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="250" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="250" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A250"/>
       <c r="B250" s="2" t="s">
         <v>50</v>
@@ -11501,7 +11510,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="251" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="251" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A251"/>
       <c r="B251" s="2" t="s">
         <v>50</v>
@@ -11529,7 +11538,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="252" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="252" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A252"/>
       <c r="B252" s="2" t="s">
         <v>50</v>
@@ -11557,7 +11566,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="253" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="253" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A253"/>
       <c r="B253" s="2" t="s">
         <v>50</v>
@@ -11585,7 +11594,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="254" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="254" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A254"/>
       <c r="B254" s="2" t="s">
         <v>50</v>
@@ -11607,7 +11616,7 @@
       </c>
       <c r="I254"/>
     </row>
-    <row r="255" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="255" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A255"/>
       <c r="B255" s="2" t="s">
         <v>50</v>
@@ -11629,7 +11638,7 @@
       </c>
       <c r="I255"/>
     </row>
-    <row r="256" spans="1:14" s="5" customFormat="1" hidden="1">
+    <row r="256" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A256"/>
       <c r="B256" s="2" t="s">
         <v>50</v>
@@ -11651,7 +11660,7 @@
       </c>
       <c r="I256"/>
     </row>
-    <row r="257" spans="1:11" s="5" customFormat="1" hidden="1">
+    <row r="257" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A257"/>
       <c r="B257" s="2" t="s">
         <v>50</v>
@@ -11673,7 +11682,7 @@
       </c>
       <c r="I257"/>
     </row>
-    <row r="258" spans="1:11" s="5" customFormat="1" hidden="1">
+    <row r="258" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A258"/>
       <c r="B258" s="2" t="s">
         <v>50</v>
@@ -11695,7 +11704,7 @@
       </c>
       <c r="I258"/>
     </row>
-    <row r="259" spans="1:11" s="5" customFormat="1" hidden="1">
+    <row r="259" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A259"/>
       <c r="B259" s="2" t="s">
         <v>50</v>
@@ -11717,7 +11726,7 @@
       </c>
       <c r="I259"/>
     </row>
-    <row r="260" spans="1:11" s="5" customFormat="1" hidden="1">
+    <row r="260" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A260"/>
       <c r="B260" s="2" t="s">
         <v>50</v>
@@ -11745,7 +11754,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="261" spans="1:11" s="5" customFormat="1" hidden="1">
+    <row r="261" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A261"/>
       <c r="B261" s="2" t="s">
         <v>50</v>
@@ -11767,7 +11776,7 @@
       </c>
       <c r="I261"/>
     </row>
-    <row r="262" spans="1:11" s="5" customFormat="1" hidden="1">
+    <row r="262" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A262"/>
       <c r="B262" s="2" t="s">
         <v>50</v>
@@ -11789,7 +11798,7 @@
       </c>
       <c r="I262"/>
     </row>
-    <row r="263" spans="1:11" s="5" customFormat="1" hidden="1">
+    <row r="263" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A263"/>
       <c r="B263" s="2" t="s">
         <v>50</v>
@@ -11811,7 +11820,7 @@
       </c>
       <c r="I263"/>
     </row>
-    <row r="264" spans="1:11" s="5" customFormat="1" hidden="1">
+    <row r="264" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A264"/>
       <c r="B264" s="2" t="s">
         <v>50</v>
@@ -11833,7 +11842,7 @@
       </c>
       <c r="I264"/>
     </row>
-    <row r="265" spans="1:11" s="5" customFormat="1" hidden="1">
+    <row r="265" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A265"/>
       <c r="B265" s="2" t="s">
         <v>50</v>
@@ -11855,7 +11864,7 @@
       </c>
       <c r="I265"/>
     </row>
-    <row r="266" spans="1:11" s="5" customFormat="1" hidden="1">
+    <row r="266" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A266"/>
       <c r="B266" s="2" t="s">
         <v>50</v>
@@ -11883,7 +11892,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="267" spans="1:11" s="5" customFormat="1" hidden="1">
+    <row r="267" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A267"/>
       <c r="B267" s="2" t="s">
         <v>50</v>
@@ -11911,7 +11920,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="268" spans="1:11" s="5" customFormat="1" hidden="1">
+    <row r="268" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A268"/>
       <c r="B268" s="2" t="s">
         <v>50</v>
@@ -11939,7 +11948,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="269" spans="1:11" s="5" customFormat="1" hidden="1">
+    <row r="269" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A269"/>
       <c r="B269" s="2" t="s">
         <v>50</v>
@@ -11967,7 +11976,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="270" spans="1:11" s="5" customFormat="1" hidden="1">
+    <row r="270" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A270"/>
       <c r="B270" s="2" t="s">
         <v>50</v>
@@ -11995,7 +12004,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="271" spans="1:11" s="5" customFormat="1" hidden="1">
+    <row r="271" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A271"/>
       <c r="B271" s="2" t="s">
         <v>50</v>
@@ -12023,7 +12032,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="272" spans="1:11" s="5" customFormat="1" hidden="1">
+    <row r="272" spans="1:11" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A272"/>
       <c r="B272" s="2" t="s">
         <v>50</v>
@@ -12051,7 +12060,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="273" spans="1:29" s="5" customFormat="1">
+    <row r="273" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>114</v>
       </c>
@@ -12078,7 +12087,7 @@
       </c>
       <c r="I273"/>
       <c r="J273" s="5" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K273" s="5">
         <v>11</v>
@@ -12138,7 +12147,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="274" spans="1:29" s="5" customFormat="1" hidden="1">
+    <row r="274" spans="1:29" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A274"/>
       <c r="B274" s="2" t="s">
         <v>50</v>
@@ -12166,7 +12175,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="275" spans="1:29" s="5" customFormat="1" hidden="1">
+    <row r="275" spans="1:29" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A275"/>
       <c r="B275" s="2" t="s">
         <v>50</v>
@@ -12188,7 +12197,7 @@
       </c>
       <c r="I275"/>
     </row>
-    <row r="276" spans="1:29" hidden="1">
+    <row r="276" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="B276" s="2" t="s">
         <v>50</v>
       </c>
@@ -12211,7 +12220,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="277" spans="1:29" hidden="1">
+    <row r="277" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="B277" s="2" t="s">
         <v>50</v>
       </c>
@@ -12234,7 +12243,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="278" spans="1:29">
+    <row r="278" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>115</v>
       </c>
@@ -12260,7 +12269,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="279" spans="1:29" s="5" customFormat="1" hidden="1">
+    <row r="279" spans="1:29" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A279"/>
       <c r="B279" s="2" t="s">
         <v>50</v>
@@ -12282,7 +12291,7 @@
       </c>
       <c r="I279"/>
     </row>
-    <row r="280" spans="1:29" s="5" customFormat="1" hidden="1">
+    <row r="280" spans="1:29" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A280"/>
       <c r="B280" s="2" t="s">
         <v>50</v>
@@ -12304,7 +12313,7 @@
       </c>
       <c r="I280"/>
     </row>
-    <row r="281" spans="1:29" s="5" customFormat="1" hidden="1">
+    <row r="281" spans="1:29" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A281"/>
       <c r="B281" s="2" t="s">
         <v>50</v>
@@ -12326,7 +12335,7 @@
       </c>
       <c r="I281"/>
     </row>
-    <row r="282" spans="1:29" ht="25.5">
+    <row r="282" spans="1:29" ht="34" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>116</v>
       </c>
@@ -12352,7 +12361,7 @@
         <v>459</v>
       </c>
       <c r="J282" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K282" s="11">
         <v>11</v>
@@ -12367,7 +12376,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="283" spans="1:29" s="5" customFormat="1" hidden="1">
+    <row r="283" spans="1:29" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A283"/>
       <c r="B283" s="2" t="s">
         <v>50</v>
@@ -12395,7 +12404,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="284" spans="1:29" s="5" customFormat="1" hidden="1">
+    <row r="284" spans="1:29" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A284"/>
       <c r="B284" s="2" t="s">
         <v>50</v>
@@ -12423,7 +12432,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="285" spans="1:29" s="5" customFormat="1">
+    <row r="285" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A285"/>
       <c r="B285" s="2" t="s">
         <v>50</v>
@@ -12445,7 +12454,7 @@
       </c>
       <c r="I285"/>
     </row>
-    <row r="286" spans="1:29" s="5" customFormat="1" hidden="1">
+    <row r="286" spans="1:29" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A286"/>
       <c r="B286" s="2" t="s">
         <v>50</v>
@@ -12467,7 +12476,7 @@
       </c>
       <c r="I286"/>
     </row>
-    <row r="287" spans="1:29" s="5" customFormat="1" hidden="1">
+    <row r="287" spans="1:29" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A287"/>
       <c r="B287" s="2" t="s">
         <v>50</v>
@@ -12489,7 +12498,7 @@
       </c>
       <c r="I287"/>
     </row>
-    <row r="288" spans="1:29" s="5" customFormat="1">
+    <row r="288" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A288"/>
       <c r="B288" s="2" t="s">
         <v>50</v>
@@ -12511,7 +12520,7 @@
       </c>
       <c r="I288"/>
     </row>
-    <row r="289" spans="1:19" s="5" customFormat="1">
+    <row r="289" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A289"/>
       <c r="B289" s="2" t="s">
         <v>50</v>
@@ -12533,7 +12542,7 @@
       </c>
       <c r="I289"/>
     </row>
-    <row r="290" spans="1:19" s="5" customFormat="1" hidden="1">
+    <row r="290" spans="1:19" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A290"/>
       <c r="B290" s="2" t="s">
         <v>50</v>
@@ -12561,7 +12570,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="291" spans="1:19" s="5" customFormat="1" hidden="1">
+    <row r="291" spans="1:19" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A291"/>
       <c r="B291" s="2" t="s">
         <v>50</v>
@@ -12589,7 +12598,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="292" spans="1:19" s="5" customFormat="1" hidden="1">
+    <row r="292" spans="1:19" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A292"/>
       <c r="B292" s="2" t="s">
         <v>50</v>
@@ -12617,7 +12626,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="293" spans="1:19" s="5" customFormat="1" hidden="1">
+    <row r="293" spans="1:19" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A293"/>
       <c r="B293" s="2" t="s">
         <v>50</v>
@@ -12639,7 +12648,7 @@
       </c>
       <c r="I293"/>
     </row>
-    <row r="294" spans="1:19" s="5" customFormat="1">
+    <row r="294" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>117</v>
       </c>
@@ -12666,7 +12675,7 @@
       </c>
       <c r="I294"/>
       <c r="J294" s="5" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K294" s="5">
         <v>11</v>
@@ -12696,7 +12705,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="295" spans="1:19" customFormat="1">
+    <row r="295" spans="1:19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B295" s="2" t="s">
         <v>50</v>
       </c>
@@ -12708,7 +12717,7 @@
       <c r="G295" s="1"/>
       <c r="H295" s="3"/>
     </row>
-    <row r="296" spans="1:19" ht="25.5">
+    <row r="296" spans="1:19" ht="34" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>118</v>
       </c>
@@ -12734,7 +12743,7 @@
         <v>588</v>
       </c>
       <c r="J296" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K296" s="11">
         <v>11</v>
@@ -12743,7 +12752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:19" hidden="1">
+    <row r="297" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="B297" s="2" t="s">
         <v>50</v>
       </c>
@@ -12766,7 +12775,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="298" spans="1:19">
+    <row r="298" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>119</v>
       </c>
@@ -12792,7 +12801,7 @@
         <v>589</v>
       </c>
       <c r="J298" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K298" s="11">
         <v>11</v>
@@ -12801,7 +12810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:19" ht="25.5">
+    <row r="299" spans="1:19" ht="34" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>120</v>
       </c>
@@ -12827,7 +12836,7 @@
         <v>590</v>
       </c>
       <c r="J299" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K299" s="11">
         <v>11</v>
@@ -12848,7 +12857,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="300" spans="1:19" s="5" customFormat="1">
+    <row r="300" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>121</v>
       </c>
@@ -12875,7 +12884,7 @@
       </c>
       <c r="I300"/>
     </row>
-    <row r="301" spans="1:19" hidden="1">
+    <row r="301" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="B301" s="2" t="s">
         <v>50</v>
       </c>
@@ -12898,7 +12907,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="302" spans="1:19" s="5" customFormat="1" ht="38.25">
+    <row r="302" spans="1:19" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.3">
       <c r="A302">
         <v>122</v>
       </c>
@@ -12925,7 +12934,7 @@
       </c>
       <c r="I302"/>
       <c r="J302" s="5" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K302" s="5">
         <v>11</v>
@@ -12949,7 +12958,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="303" spans="1:19" hidden="1">
+    <row r="303" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
       <c r="B303" s="2" t="s">
         <v>50</v>
       </c>
@@ -12972,7 +12981,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="304" spans="1:19">
+    <row r="304" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A304">
         <v>123</v>
       </c>
@@ -12998,7 +13007,7 @@
         <v>595</v>
       </c>
       <c r="J304" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K304" s="11">
         <v>11</v>
@@ -13010,7 +13019,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="305" spans="1:16" hidden="1">
+    <row r="305" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="B305" s="2" t="s">
         <v>50</v>
       </c>
@@ -13033,7 +13042,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="306" spans="1:16">
+    <row r="306" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A306">
         <v>124</v>
       </c>
@@ -13059,7 +13068,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="307" spans="1:16">
+    <row r="307" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A307">
         <v>125</v>
       </c>
@@ -13085,7 +13094,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="308" spans="1:16" hidden="1">
+    <row r="308" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="B308" s="2" t="s">
         <v>50</v>
       </c>
@@ -13108,7 +13117,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="309" spans="1:16" s="5" customFormat="1">
+    <row r="309" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A309">
         <v>126</v>
       </c>
@@ -13135,13 +13144,13 @@
       </c>
       <c r="I309"/>
       <c r="J309" s="5" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K309" s="5">
         <v>11</v>
       </c>
     </row>
-    <row r="310" spans="1:16" s="5" customFormat="1">
+    <row r="310" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A310">
         <v>127</v>
       </c>
@@ -13168,7 +13177,7 @@
       </c>
       <c r="I310"/>
       <c r="J310" s="5" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K310" s="5">
         <v>11</v>
@@ -13177,7 +13186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:16" ht="38.25">
+    <row r="311" spans="1:16" ht="51" x14ac:dyDescent="0.3">
       <c r="A311">
         <v>128</v>
       </c>
@@ -13203,7 +13212,7 @@
         <v>592</v>
       </c>
       <c r="J311" s="11" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K311" s="11">
         <v>11</v>
@@ -13221,7 +13230,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="312" spans="1:16">
+    <row r="312" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A312">
         <v>129</v>
       </c>
@@ -13247,7 +13256,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="313" spans="1:16">
+    <row r="313" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A313">
         <v>130</v>
       </c>
@@ -13273,7 +13282,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="314" spans="1:16" s="5" customFormat="1">
+    <row r="314" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A314" s="5">
         <v>131</v>
       </c>
@@ -13299,7 +13308,7 @@
         <v>568</v>
       </c>
       <c r="J314" s="5" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="K314" s="5">
         <v>11</v>
@@ -13320,7 +13329,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="315" spans="1:16" s="5" customFormat="1">
+    <row r="315" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A315">
         <v>132</v>
       </c>
@@ -13347,7 +13356,7 @@
       </c>
       <c r="I315"/>
     </row>
-    <row r="316" spans="1:16" hidden="1">
+    <row r="316" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A316">
         <v>133</v>
       </c>
@@ -13370,7 +13379,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="317" spans="1:16" s="5" customFormat="1" hidden="1">
+    <row r="317" spans="1:16" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A317">
         <v>134</v>
       </c>
@@ -13394,7 +13403,7 @@
       </c>
       <c r="I317"/>
     </row>
-    <row r="318" spans="1:16" customFormat="1">
+    <row r="318" spans="1:16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A318">
         <v>135</v>
       </c>
@@ -13409,7 +13418,7 @@
       <c r="G318" s="1"/>
       <c r="H318" s="3"/>
     </row>
-    <row r="319" spans="1:16" customFormat="1">
+    <row r="319" spans="1:16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B319" s="2" t="s">
         <v>50</v>
       </c>
@@ -13421,7 +13430,7 @@
       <c r="G319" s="1"/>
       <c r="H319" s="3"/>
     </row>
-    <row r="320" spans="1:16" customFormat="1">
+    <row r="320" spans="1:16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B320" s="2" t="s">
         <v>50</v>
       </c>
@@ -13433,7 +13442,7 @@
       <c r="G320" s="1"/>
       <c r="H320" s="3"/>
     </row>
-    <row r="321" spans="1:8" customFormat="1">
+    <row r="321" spans="1:8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B321" s="2" t="s">
         <v>50</v>
       </c>
@@ -13445,7 +13454,7 @@
       <c r="G321" s="1"/>
       <c r="H321" s="3"/>
     </row>
-    <row r="322" spans="1:8" customFormat="1">
+    <row r="322" spans="1:8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A322">
         <v>136</v>
       </c>
@@ -13461,7 +13470,7 @@
       <c r="H322" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AC322">
+  <autoFilter ref="A1:AC322" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="7">
       <customFilters>
         <customFilter operator="notEqual" val="*a*"/>

</xml_diff>